<commit_message>
Update to June schedule
</commit_message>
<xml_diff>
--- a/2024 Agile 103 Class Calendar-4-11.xlsx
+++ b/2024 Agile 103 Class Calendar-4-11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPMC\Documents\GitHub\agile103-calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5108AB7-5277-4781-88AF-53FD38712FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C364C81-4CF3-4D24-AED6-BCEF68BB2368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="726" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2074,35 +2074,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>7:00 PM - 9:00 PM EST</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Interview workshop</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="14"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -2230,75 +2201,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">2:00 PM - 4:00 PM EST </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
-Different Environments in Software Dev</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">2:00 PM - 4:00 PM EST </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
-Simulation (Sprint Planning)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>7:00 PM - 9:00 PM EST</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Simulation (Backlog Refinement)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -2323,26 +2225,6 @@
       </rPr>
       <t xml:space="preserve">
 Simulation (Sprint Demo &amp; DSU)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">2:00 PM - 4:00 PM EST </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
-Simulation (Sprint Retrospetive)</t>
     </r>
   </si>
   <si>
@@ -2494,6 +2376,155 @@
         <family val="2"/>
       </rPr>
       <t>Guest Speaker</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2:00 PM - 4:00 PM EST </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Different Environments in Software Dev
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Guest Speaker</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>7:00 PM - 9:00 PM EST</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Simulation (Sprint Retrospetive)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2:00 PM - 4:00 PM EST </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Simulation (Sprint Planning) + Backlog Refinement</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2:00 PM - 4:00 PM EST </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Class Cancelled</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>7:00 PM - 9:00 PM EST</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Open Discussion</t>
     </r>
   </si>
 </sst>
@@ -3632,10 +3663,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6159,7 +6186,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="63" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6240,7 +6267,7 @@
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="40" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6268,19 +6295,19 @@
     </row>
     <row r="6" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="40" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="40" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F6" s="25"/>
       <c r="G6" s="40" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6308,11 +6335,11 @@
     </row>
     <row r="8" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="25"/>
+        <v>133</v>
+      </c>
+      <c r="B8" s="40"/>
       <c r="C8" s="40" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="40" t="s">
@@ -6320,7 +6347,7 @@
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6352,17 +6379,17 @@
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="40" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="40" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6391,21 +6418,21 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="104.4" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>138</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="40" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.25">
@@ -6433,19 +6460,19 @@
     </row>
     <row r="14" spans="1:12" ht="97.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -6545,15 +6572,15 @@
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -6581,7 +6608,7 @@
     </row>
     <row r="6" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>

</xml_diff>